<commit_message>
Update Modules - Create MB21
</commit_message>
<xml_diff>
--- a/Archivo_Creación.xlsx
+++ b/Archivo_Creación.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpdhl.sharepoint.com/teams/ContinuousImprovement_Tech/Shared Documents/eDOCS/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bleonpar\OneDrive - DPDHL\Desktop\LionOps_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{B2C04B44-4888-4D56-8804-904A30030E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD062C0-570A-4B99-9FED-D974F9F653F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29102ED-4964-4D7E-9B79-583537DFEADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{ED75A33F-D1E2-485B-968B-A9C4E86322F3}"/>
   </bookViews>
@@ -267,7 +267,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,16 +320,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -356,7 +359,274 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -434,311 +704,13 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -783,6 +755,37 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -999,18 +1002,18 @@
     <tableColumn id="1" xr3:uid="{AA341CC6-2985-4570-AD63-EFBF8A6975FC}" name="INDICE" dataDxfId="14"/>
     <tableColumn id="19" xr3:uid="{531143DF-3FE0-4D3F-9D17-03AB2D4DED6D}" name="PEDIDO" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{938E4908-4A83-48CB-9ECE-C0E0BA307318}" name="ENTREGA" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{87DA9F48-A4C0-4054-9569-1B7D1D341D38}" name="PROYECTO" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{7BDA59EB-8D01-4D6A-9C81-FF5840FD8969}" name="MATERIAL" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{DFC01692-8136-4C43-82D7-B6CDA142A486}" name="CANTIDAD" dataDxfId="0" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{ABB7AD40-1422-4BCC-B6B1-41BFB09FCBE1}" name="FECHA" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{8AFDC736-2616-4EDF-AD55-9B1230BFFD1F}" name="CENTRO" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="14" xr3:uid="{48B8E408-4B66-438F-99EB-4DA75D609C00}" name="ALM.DEST" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{64289AE3-9D91-45AD-B8EB-AA3230203BDE}" name="LOTE" dataDxfId="8" dataCellStyle="Millares 11"/>
-    <tableColumn id="22" xr3:uid="{7417BA8F-F1A5-41A3-936D-A0D512306987}" name="OT" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{7A613780-E9B8-4C33-AC1A-A707916E5094}" name="BODEGA" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{78E79FE1-6553-4A4F-B382-AE0C2ADD6CC2}" name="PEP" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{A9E07D31-55C0-425F-AA81-7673B43F13F9}" name="CLASE DE MOV" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{AF62E663-6ED2-4102-8037-1AD26DCFC497}" name="GUARDAR" dataDxfId="6">
+    <tableColumn id="9" xr3:uid="{87DA9F48-A4C0-4054-9569-1B7D1D341D38}" name="PROYECTO" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{7BDA59EB-8D01-4D6A-9C81-FF5840FD8969}" name="MATERIAL" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{DFC01692-8136-4C43-82D7-B6CDA142A486}" name="CANTIDAD" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{ABB7AD40-1422-4BCC-B6B1-41BFB09FCBE1}" name="FECHA" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{8AFDC736-2616-4EDF-AD55-9B1230BFFD1F}" name="CENTRO" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="14" xr3:uid="{48B8E408-4B66-438F-99EB-4DA75D609C00}" name="ALM.DEST" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{64289AE3-9D91-45AD-B8EB-AA3230203BDE}" name="LOTE" dataDxfId="5" dataCellStyle="Millares 11"/>
+    <tableColumn id="22" xr3:uid="{7417BA8F-F1A5-41A3-936D-A0D512306987}" name="OT" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{7A613780-E9B8-4C33-AC1A-A707916E5094}" name="BODEGA" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{78E79FE1-6553-4A4F-B382-AE0C2ADD6CC2}" name="PEP" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A9E07D31-55C0-425F-AA81-7673B43F13F9}" name="CLASE DE MOV" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{AF62E663-6ED2-4102-8037-1AD26DCFC497}" name="GUARDAR" dataDxfId="1">
       <calculatedColumnFormula>IF(AND(OR(A2="I",A2="A"),A3="X"),"X","")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1339,7 +1342,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,7 +1409,7 @@
       <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="20" t="s">
         <v>22</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -1425,13 +1428,13 @@
       <c r="E2" s="14">
         <v>1020328</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="19">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -1447,7 +1450,7 @@
         <v>9</v>
       </c>
       <c r="M2" s="13"/>
-      <c r="N2" s="18">
+      <c r="N2" s="21">
         <v>221</v>
       </c>
       <c r="O2" s="6"/>
@@ -1462,13 +1465,13 @@
       <c r="E3" s="14">
         <v>1020328</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1484,7 +1487,7 @@
         <v>19</v>
       </c>
       <c r="M3" s="13"/>
-      <c r="N3" s="18">
+      <c r="N3" s="21">
         <v>221</v>
       </c>
       <c r="O3" s="6"/>
@@ -1499,13 +1502,13 @@
       <c r="E4" s="14">
         <v>4022443</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="19">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -1521,7 +1524,7 @@
         <v>19</v>
       </c>
       <c r="M4" s="13"/>
-      <c r="N4" s="18">
+      <c r="N4" s="21">
         <v>221</v>
       </c>
       <c r="O4" s="6"/>
@@ -1536,13 +1539,13 @@
       <c r="E5" s="14">
         <v>4043352</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="19">
         <v>4</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -1558,7 +1561,7 @@
         <v>19</v>
       </c>
       <c r="M5" s="13"/>
-      <c r="N5" s="18">
+      <c r="N5" s="21">
         <v>221</v>
       </c>
       <c r="O5" s="6"/>
@@ -1573,13 +1576,13 @@
       <c r="E6" s="14">
         <v>4055581</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>5</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1595,7 +1598,7 @@
         <v>19</v>
       </c>
       <c r="M6" s="13"/>
-      <c r="N6" s="18">
+      <c r="N6" s="21">
         <v>221</v>
       </c>
       <c r="O6" s="6"/>
@@ -1610,13 +1613,13 @@
       <c r="E7" s="14">
         <v>4059049</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -1632,7 +1635,7 @@
         <v>19</v>
       </c>
       <c r="M7" s="13"/>
-      <c r="N7" s="18">
+      <c r="N7" s="21">
         <v>221</v>
       </c>
       <c r="O7" s="8"/>
@@ -1647,13 +1650,13 @@
       <c r="E8" s="14">
         <v>1020328</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>7</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="6" t="s">
@@ -1669,7 +1672,7 @@
         <v>9</v>
       </c>
       <c r="M8" s="13"/>
-      <c r="N8" s="18">
+      <c r="N8" s="21">
         <v>221</v>
       </c>
       <c r="O8" s="8"/>
@@ -1684,13 +1687,13 @@
       <c r="E9" s="14">
         <v>4059049</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>8</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -1706,7 +1709,7 @@
         <v>19</v>
       </c>
       <c r="M9" s="13"/>
-      <c r="N9" s="18">
+      <c r="N9" s="21">
         <v>221</v>
       </c>
       <c r="O9" s="8"/>
@@ -1721,13 +1724,13 @@
       <c r="E10" s="14">
         <v>4022443</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="19">
         <v>9</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -1743,7 +1746,7 @@
         <v>19</v>
       </c>
       <c r="M10" s="13"/>
-      <c r="N10" s="18">
+      <c r="N10" s="21">
         <v>221</v>
       </c>
       <c r="O10" s="8"/>
@@ -1758,13 +1761,13 @@
       <c r="E11" s="14">
         <v>4043352</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="19">
         <v>10</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1780,7 +1783,7 @@
         <v>19</v>
       </c>
       <c r="M11" s="13"/>
-      <c r="N11" s="18">
+      <c r="N11" s="21">
         <v>221</v>
       </c>
       <c r="O11" s="8"/>
@@ -1795,13 +1798,13 @@
       <c r="E12" s="14">
         <v>4055581</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>11</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="6" t="s">
@@ -1817,7 +1820,7 @@
         <v>19</v>
       </c>
       <c r="M12" s="13"/>
-      <c r="N12" s="18">
+      <c r="N12" s="21">
         <v>221</v>
       </c>
       <c r="O12" s="8"/>
@@ -1832,13 +1835,13 @@
       <c r="E13" s="14">
         <v>4059049</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <v>12</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -1854,7 +1857,7 @@
         <v>19</v>
       </c>
       <c r="M13" s="13"/>
-      <c r="N13" s="18">
+      <c r="N13" s="21">
         <v>221</v>
       </c>
       <c r="O13" s="8"/>
@@ -1869,13 +1872,13 @@
       <c r="E14" s="14">
         <v>1020328</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="19">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -1891,7 +1894,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="13"/>
-      <c r="N14" s="18">
+      <c r="N14" s="21">
         <v>221</v>
       </c>
       <c r="O14" s="6"/>
@@ -1906,13 +1909,13 @@
       <c r="E15" s="14">
         <v>4059049</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="19">
         <v>14</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -1928,7 +1931,7 @@
         <v>19</v>
       </c>
       <c r="M15" s="13"/>
-      <c r="N15" s="18">
+      <c r="N15" s="21">
         <v>221</v>
       </c>
       <c r="O15" s="6"/>
@@ -1943,13 +1946,13 @@
       <c r="E16" s="14">
         <v>4043352</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="19">
         <v>15</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -1965,7 +1968,7 @@
         <v>19</v>
       </c>
       <c r="M16" s="13"/>
-      <c r="N16" s="18">
+      <c r="N16" s="21">
         <v>221</v>
       </c>
       <c r="O16" s="8"/>
@@ -1980,13 +1983,13 @@
       <c r="E17" s="14">
         <v>4059049</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="19">
         <v>16</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -2002,7 +2005,7 @@
         <v>19</v>
       </c>
       <c r="M17" s="13"/>
-      <c r="N17" s="18">
+      <c r="N17" s="21">
         <v>221</v>
       </c>
       <c r="O17" s="8"/>
@@ -2017,13 +2020,13 @@
       <c r="E18" s="14">
         <v>4043352</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="19">
         <v>17</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -2039,7 +2042,7 @@
         <v>19</v>
       </c>
       <c r="M18" s="13"/>
-      <c r="N18" s="18">
+      <c r="N18" s="21">
         <v>221</v>
       </c>
       <c r="O18" s="8"/>
@@ -2054,13 +2057,13 @@
       <c r="E19" s="14">
         <v>4059049</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="19">
         <v>18</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="6" t="s">
@@ -2076,7 +2079,7 @@
         <v>19</v>
       </c>
       <c r="M19" s="13"/>
-      <c r="N19" s="18">
+      <c r="N19" s="21">
         <v>221</v>
       </c>
       <c r="O19" s="8"/>
@@ -2091,13 +2094,13 @@
       <c r="E20" s="14">
         <v>4043352</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="19">
         <v>19</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="6" t="s">
@@ -2113,7 +2116,7 @@
         <v>19</v>
       </c>
       <c r="M20" s="13"/>
-      <c r="N20" s="18">
+      <c r="N20" s="21">
         <v>221</v>
       </c>
       <c r="O20" s="8"/>
@@ -2128,13 +2131,13 @@
       <c r="E21" s="14">
         <v>4043352</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="19">
         <v>20</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -2150,7 +2153,7 @@
         <v>19</v>
       </c>
       <c r="M21" s="15"/>
-      <c r="N21" s="19">
+      <c r="N21" s="22">
         <v>221</v>
       </c>
       <c r="O21" s="12"/>
@@ -2165,13 +2168,13 @@
       <c r="E22" s="14">
         <v>4043352</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="19">
         <v>21</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -2187,7 +2190,7 @@
         <v>19</v>
       </c>
       <c r="M22" s="15"/>
-      <c r="N22" s="19">
+      <c r="N22" s="22">
         <v>221</v>
       </c>
       <c r="O22" s="12"/>
@@ -2202,13 +2205,13 @@
       <c r="E23" s="14">
         <v>4043352</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="19">
         <v>22</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -2224,7 +2227,7 @@
         <v>19</v>
       </c>
       <c r="M23" s="15"/>
-      <c r="N23" s="19">
+      <c r="N23" s="22">
         <v>221</v>
       </c>
       <c r="O23" s="12"/>
@@ -2239,13 +2242,13 @@
       <c r="E24" s="14">
         <v>4043352</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="19">
         <v>23</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -2261,7 +2264,7 @@
         <v>19</v>
       </c>
       <c r="M24" s="15"/>
-      <c r="N24" s="19">
+      <c r="N24" s="22">
         <v>221</v>
       </c>
       <c r="O24" s="12"/>
@@ -2276,13 +2279,13 @@
       <c r="E25" s="14">
         <v>4043352</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="19">
         <v>24</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -2298,7 +2301,7 @@
         <v>19</v>
       </c>
       <c r="M25" s="15"/>
-      <c r="N25" s="19">
+      <c r="N25" s="22">
         <v>221</v>
       </c>
       <c r="O25" s="12"/>
@@ -2313,13 +2316,13 @@
       <c r="E26" s="14">
         <v>4043352</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="19">
         <v>25</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -2335,7 +2338,7 @@
         <v>19</v>
       </c>
       <c r="M26" s="15"/>
-      <c r="N26" s="19">
+      <c r="N26" s="22">
         <v>221</v>
       </c>
       <c r="O26" s="12"/>
@@ -2350,13 +2353,13 @@
       <c r="E27" s="14">
         <v>4043352</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="19">
         <v>26</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -2372,7 +2375,7 @@
         <v>19</v>
       </c>
       <c r="M27" s="15"/>
-      <c r="N27" s="19">
+      <c r="N27" s="22">
         <v>221</v>
       </c>
       <c r="O27" s="12"/>
@@ -2387,13 +2390,13 @@
       <c r="E28" s="14">
         <v>4043352</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="19">
         <v>27</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -2409,7 +2412,7 @@
         <v>19</v>
       </c>
       <c r="M28" s="15"/>
-      <c r="N28" s="19">
+      <c r="N28" s="22">
         <v>221</v>
       </c>
       <c r="O28" s="12"/>
@@ -2424,13 +2427,13 @@
       <c r="E29" s="14">
         <v>4043352</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="19">
         <v>28</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="6" t="s">
@@ -2446,7 +2449,7 @@
         <v>19</v>
       </c>
       <c r="M29" s="15"/>
-      <c r="N29" s="19">
+      <c r="N29" s="22">
         <v>221</v>
       </c>
       <c r="O29" s="12"/>
@@ -2461,13 +2464,13 @@
       <c r="E30" s="14">
         <v>4043352</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="19">
         <v>29</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I30" s="6" t="s">
@@ -2483,7 +2486,7 @@
         <v>19</v>
       </c>
       <c r="M30" s="15"/>
-      <c r="N30" s="19">
+      <c r="N30" s="22">
         <v>221</v>
       </c>
       <c r="O30" s="12"/>
@@ -2498,13 +2501,13 @@
       <c r="E31" s="14">
         <v>4043352</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="19">
         <v>30</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I31" s="6" t="s">
@@ -2520,7 +2523,7 @@
         <v>19</v>
       </c>
       <c r="M31" s="15"/>
-      <c r="N31" s="19">
+      <c r="N31" s="22">
         <v>221</v>
       </c>
       <c r="O31" s="12"/>
@@ -2535,13 +2538,13 @@
       <c r="E32" s="14">
         <v>4043352</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="19">
         <v>31</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I32" s="6" t="s">
@@ -2557,7 +2560,7 @@
         <v>19</v>
       </c>
       <c r="M32" s="15"/>
-      <c r="N32" s="19">
+      <c r="N32" s="22">
         <v>221</v>
       </c>
       <c r="O32" s="12"/>
@@ -2572,13 +2575,13 @@
       <c r="E33" s="14">
         <v>4043352</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="19">
         <v>32</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I33" s="6" t="s">
@@ -2594,7 +2597,7 @@
         <v>19</v>
       </c>
       <c r="M33" s="15"/>
-      <c r="N33" s="19">
+      <c r="N33" s="22">
         <v>221</v>
       </c>
       <c r="O33" s="12"/>
@@ -2609,13 +2612,13 @@
       <c r="E34" s="14">
         <v>4043352</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="19">
         <v>33</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I34" s="6" t="s">
@@ -2631,7 +2634,7 @@
         <v>19</v>
       </c>
       <c r="M34" s="15"/>
-      <c r="N34" s="19">
+      <c r="N34" s="22">
         <v>221</v>
       </c>
       <c r="O34" s="12"/>
@@ -2646,13 +2649,13 @@
       <c r="E35" s="14">
         <v>4043352</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="19">
         <v>34</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I35" s="6" t="s">
@@ -2668,7 +2671,7 @@
         <v>19</v>
       </c>
       <c r="M35" s="15"/>
-      <c r="N35" s="19">
+      <c r="N35" s="22">
         <v>221</v>
       </c>
       <c r="O35" s="12"/>
@@ -2683,13 +2686,13 @@
       <c r="E36" s="14">
         <v>4043352</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="19">
         <v>35</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="6" t="s">
@@ -2705,7 +2708,7 @@
         <v>19</v>
       </c>
       <c r="M36" s="15"/>
-      <c r="N36" s="19">
+      <c r="N36" s="22">
         <v>221</v>
       </c>
       <c r="O36" s="12"/>
@@ -2720,13 +2723,13 @@
       <c r="E37" s="14">
         <v>4043352</v>
       </c>
-      <c r="F37" s="21">
+      <c r="F37" s="19">
         <v>36</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="18" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="6" t="s">
@@ -2742,7 +2745,7 @@
         <v>19</v>
       </c>
       <c r="M37" s="15"/>
-      <c r="N37" s="19">
+      <c r="N37" s="22">
         <v>221</v>
       </c>
       <c r="O37" s="12" t="s">
@@ -2759,26 +2762,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="93468230-7e6d-43c9-9d37-006396450f9e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c9af5c9-7ce3-46ab-a9f2-5d64e458dcf3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100575106F7B681D94693567A49D482ED10" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="801bc0e31de97ccf15b16356df39b5fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c9af5c9-7ce3-46ab-a9f2-5d64e458dcf3" xmlns:ns3="93468230-7e6d-43c9-9d37-006396450f9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8135ca6834f3b31dd78ce90ce6f9c872" ns2:_="" ns3:_="">
     <xsd:import namespace="4c9af5c9-7ce3-46ab-a9f2-5d64e458dcf3"/>
@@ -2967,10 +2950,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="93468230-7e6d-43c9-9d37-006396450f9e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c9af5c9-7ce3-46ab-a9f2-5d64e458dcf3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81724736-A986-4AC4-9EA4-EC93B9D519DB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8398244-4423-4332-8E19-130D60478A7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4c9af5c9-7ce3-46ab-a9f2-5d64e458dcf3"/>
+    <ds:schemaRef ds:uri="93468230-7e6d-43c9-9d37-006396450f9e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2987,7 +3001,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8398244-4423-4332-8E19-130D60478A7D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81724736-A986-4AC4-9EA4-EC93B9D519DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>